<commit_message>
Added Epics under Components
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Austin-Issues.xlsx
+++ b/blueprint-jira-better-excel/Austin-Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702B4288-785E-4BE2-B0DD-EE316CCDCA86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB0DACE-F2A0-4A49-9CCB-7EF8A0A3C5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId6"/>
+    <pivotCache cacheId="52" r:id="rId6"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1307,7 +1307,52 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -1348,7 +1393,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44103.619389814812" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44111.411926851855" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -1368,7 +1413,11 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Summary" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsBlank="1" count="3">
+        <s v="&lt;jt:hyperlink address=&quot;${requestContext.canonicalBaseUrl}/browse/${issue.key}&quot; value=&quot;${issue.summary}&quot;/&gt;"/>
+        <m/>
+        <s v="NEEDS FOR FILTERING IN PIVOT TABLES"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Team" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1573,12 +1622,11 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Release #" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="11.3" maxValue="11.5" count="5">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="11.3" maxValue="11.4" count="4">
         <s v="${fieldHelper.getFieldValueByName(issue, &quot;Release #&quot;)}"/>
         <m/>
+        <n v="11.4"/>
         <n v="11.3"/>
-        <n v="11.4"/>
-        <n v="11.5"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Quality Score" numFmtId="0">
@@ -1601,7 +1649,7 @@
   <r>
     <s v="&lt;jt:forEach items=&quot;${issues}&quot; var=&quot;issue&quot;&gt;&lt;jt:hyperlink address=&quot;${requestContext.canonicalBaseUrl}/browse/${issue.key}&quot; value=&quot;${issue.key}&quot;/&gt;"/>
     <x v="0"/>
-    <s v="&lt;jt:hyperlink address=&quot;${requestContext.canonicalBaseUrl}/browse/${issue.key}&quot; value=&quot;${issue.summary}&quot;/&gt;"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <s v="${bpHelper.getCollectionField(issue, &quot;Sprint&quot;)}"/>
@@ -1644,7 +1692,7 @@
   <r>
     <s v="&lt;jt:forEach items=&quot;${issues.subList(0, 0)}&quot; var=&quot;issue&quot; where=&quot;${issue.key = ''}&quot;&gt;"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <m/>
@@ -1687,7 +1735,7 @@
   <r>
     <s v="key"/>
     <x v="2"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="2"/>
     <m/>
@@ -1730,7 +1778,7 @@
   <r>
     <s v="key"/>
     <x v="3"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="3"/>
     <m/>
@@ -1767,13 +1815,13 @@
     <m/>
     <x v="2"/>
     <x v="2"/>
-    <x v="3"/>
+    <x v="2"/>
     <s v="PROD"/>
   </r>
   <r>
     <s v="key"/>
     <x v="4"/>
-    <s v="NEEDS FOR FILTERING IN PIVOT TABLES"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="4"/>
     <m/>
@@ -1810,13 +1858,13 @@
     <m/>
     <x v="2"/>
     <x v="2"/>
-    <x v="4"/>
+    <x v="2"/>
     <m/>
   </r>
   <r>
     <s v="key"/>
     <x v="5"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="5"/>
     <m/>
@@ -1853,13 +1901,13 @@
     <m/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
+    <x v="3"/>
     <m/>
   </r>
   <r>
     <s v="key"/>
     <x v="6"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="6"/>
     <m/>
@@ -1902,7 +1950,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="3"/>
     <x v="7"/>
     <m/>
@@ -1945,7 +1993,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="8"/>
     <m/>
@@ -1988,7 +2036,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="9"/>
     <m/>
@@ -2031,7 +2079,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="4"/>
     <x v="10"/>
     <m/>
@@ -2074,7 +2122,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="11"/>
     <m/>
@@ -2117,7 +2165,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="12"/>
     <m/>
@@ -2160,7 +2208,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="13"/>
     <m/>
@@ -2203,7 +2251,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="2"/>
     <x v="14"/>
     <m/>
@@ -2246,7 +2294,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="15"/>
     <m/>
@@ -2289,7 +2337,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="16"/>
     <m/>
@@ -2332,7 +2380,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="17"/>
     <m/>
@@ -2375,7 +2423,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="18"/>
     <m/>
@@ -2418,7 +2466,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="19"/>
     <m/>
@@ -2461,7 +2509,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="20"/>
     <m/>
@@ -2504,7 +2552,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="21"/>
     <m/>
@@ -2547,7 +2595,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="22"/>
     <m/>
@@ -2590,7 +2638,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="23"/>
     <m/>
@@ -2633,7 +2681,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="24"/>
     <m/>
@@ -2676,7 +2724,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="25"/>
     <m/>
@@ -2719,7 +2767,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="26"/>
     <m/>
@@ -2762,7 +2810,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="27"/>
     <m/>
@@ -2805,7 +2853,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="28"/>
     <m/>
@@ -2848,7 +2896,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="29"/>
     <m/>
@@ -2891,7 +2939,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="30"/>
     <m/>
@@ -2934,7 +2982,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="31"/>
     <m/>
@@ -2977,7 +3025,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="32"/>
     <m/>
@@ -3020,7 +3068,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="33"/>
     <m/>
@@ -3063,7 +3111,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="34"/>
     <m/>
@@ -3106,7 +3154,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="35"/>
     <m/>
@@ -3149,7 +3197,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="36"/>
     <m/>
@@ -3192,7 +3240,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="37"/>
     <m/>
@@ -3235,7 +3283,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="38"/>
     <m/>
@@ -3278,7 +3326,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="39"/>
     <m/>
@@ -3321,7 +3369,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="40"/>
     <m/>
@@ -3364,7 +3412,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="41"/>
     <m/>
@@ -3407,7 +3455,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="42"/>
     <m/>
@@ -3450,7 +3498,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="43"/>
     <m/>
@@ -3493,7 +3541,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="44"/>
     <m/>
@@ -3536,7 +3584,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="45"/>
     <m/>
@@ -3579,7 +3627,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="46"/>
     <m/>
@@ -3622,7 +3670,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="47"/>
     <m/>
@@ -3665,7 +3713,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="48"/>
     <m/>
@@ -3708,7 +3756,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="49"/>
     <m/>
@@ -3751,7 +3799,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="50"/>
     <m/>
@@ -3794,7 +3842,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="51"/>
     <m/>
@@ -3837,7 +3885,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="52"/>
     <m/>
@@ -3880,7 +3928,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="53"/>
     <m/>
@@ -3923,7 +3971,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="54"/>
     <m/>
@@ -3966,7 +4014,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="55"/>
     <m/>
@@ -4009,7 +4057,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="56"/>
     <m/>
@@ -4052,7 +4100,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="57"/>
     <m/>
@@ -4095,7 +4143,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="58"/>
     <m/>
@@ -4138,7 +4186,7 @@
   <r>
     <s v="key"/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <m/>
@@ -4182,7 +4230,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -4316,10 +4364,9 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
-      <items count="6">
+      <items count="5">
+        <item x="3"/>
         <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
@@ -4372,7 +4419,156 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="44">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="38" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
+    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -4560,8 +4756,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -4755,8 +4951,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -4950,8 +5146,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5145,8 +5341,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5334,157 +5530,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x v="4"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="38" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
-    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
   <location ref="A7:H11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="44">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5500,7 +5547,14 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="6">
         <item x="0"/>
@@ -5519,9 +5573,9 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
       <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item t="default" sd="0"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5568,12 +5622,11 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
-      <items count="6">
+      <items count="5">
         <item x="0"/>
         <item x="1"/>
+        <item x="3"/>
         <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5582,8 +5635,9 @@
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
     <field x="10"/>
+    <field x="2"/>
   </rowFields>
   <rowItems count="2">
     <i>
@@ -5625,7 +5679,7 @@
     <pageField fld="30" hier="-1"/>
     <pageField fld="3" hier="-1"/>
     <pageField fld="37" item="0" hier="-1"/>
-    <pageField fld="39" item="2" hier="-1"/>
+    <pageField fld="39" item="3" hier="-1"/>
   </pageFields>
   <dataFields count="7">
     <dataField name="Total Estimate" fld="15" baseField="10" baseItem="1"/>
@@ -5637,7 +5691,7 @@
     <dataField name="Development Progress" fld="41" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="4">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5647,7 +5701,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5657,7 +5711,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5667,7 +5721,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5677,7 +5731,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="15">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6158,13 +6212,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -6636,7 +6690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6687,7 +6743,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="17">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -7135,7 +7191,7 @@
         <v>155</v>
       </c>
       <c r="AN4" s="5">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="AO4" s="5" t="s">
         <v>199</v>
@@ -7226,7 +7282,7 @@
         <v>155</v>
       </c>
       <c r="AN6" s="5">
-        <v>11.5</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
@@ -7264,6 +7320,9 @@
       </c>
       <c r="AM7" s="5" t="s">
         <v>155</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>11.3</v>
       </c>
     </row>
     <row r="8" spans="1:42" ht="27.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added reporting based on stories and spikes only.
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Austin-Issues.xlsx
+++ b/blueprint-jira-better-excel/Austin-Issues.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB0DACE-F2A0-4A49-9CCB-7EF8A0A3C5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3FDC45-C6EA-4DE1-82A7-5F16764C3F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
     <sheet name="Bugs" sheetId="5" r:id="rId2"/>
     <sheet name="Development" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Features" sheetId="4" r:id="rId4"/>
-    <sheet name="Issues" sheetId="2" state="hidden" r:id="rId5"/>
+    <sheet name="Features (Epics)" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Features (Stories)" sheetId="7" r:id="rId5"/>
+    <sheet name="Issues" sheetId="2" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="issues">OFFSET(Issues!$A$1,0,0,COUNTA(Issues!$A$1:$A$9999),COUNTA(Issues!$A$1:$AAL$1)-1)</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Issues!$A$1:$AS$61</definedName>
+    <definedName name="issues">OFFSET(Issues!$A$1,0,0,COUNTA(Issues!$A$1:$A$9999),COUNTA(Issues!$A$1:$AAO$1)-1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="52" r:id="rId6"/>
+    <pivotCache cacheId="224" r:id="rId7"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="213">
   <si>
     <t>Status</t>
   </si>
@@ -1057,13 +1059,49 @@
     <t>${bpHelper.isInBacklogHealth(issue)}</t>
   </si>
   <si>
-    <t>${fieldHelper.getFieldValueByName(issue, "Quality Score")}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>POC</t>
   </si>
   <si>
     <t>PROD</t>
+  </si>
+  <si>
+    <t>Story Decomposed</t>
+  </si>
+  <si>
+    <t>${fieldHelper.getFieldValueByName(issue, "Quality Score")}</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Story Decomposed SP</t>
+  </si>
+  <si>
+    <t>Story Remaining SP</t>
+  </si>
+  <si>
+    <t>${bpHelper.isStoryDecopmosed(issue)}</t>
+  </si>
+  <si>
+    <t>$[IF(AP2="Yes", N2, IF(AP2="No",0,""))]</t>
+  </si>
+  <si>
+    <t>$[IF(E2="Story: Done",0,IF(OR(B2="Story",B2="Spike"), N2, ""))]&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Decomposition Progress</t>
+  </si>
+  <si>
+    <t>Remaining Estimate (Not Closed/Not Decomposed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decomposed (Ready, In Dev, Closed) </t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1251,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1301,13 +1339,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="16">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -1316,12 +1363,6 @@
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1339,19 +1380,7 @@
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1393,11 +1422,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44111.411926851855" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44123.650799305557" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
-  <cacheFields count="44">
+  <cacheFields count="49">
     <cacheField name="Key" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -1632,9 +1661,20 @@
     <cacheField name="Quality Score" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
+    <cacheField name="Story Decomposed" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Story Decomposed SP" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Story Remaining SP" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
     <cacheField name="Component Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Epic Remaining Estimate')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
     <cacheField name="Component Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Epic Decomposed')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
     <cacheField name="Component Epic Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Stories Estimate')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
+    <cacheField name="Story Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Story Decomposed SP')/SUM('Story Points'),1)" databaseField="0"/>
+    <cacheField name="Story Development Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Story Remaining SP')/SUM('Story Points'),1)" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -1687,7 +1727,10 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <s v="${fieldHelper.getFieldValueByName(issue, &quot;Quality Score&quot;)}&lt;/jt:forEach&gt;"/>
+    <s v="${fieldHelper.getFieldValueByName(issue, &quot;Quality Score&quot;)}"/>
+    <s v="${bpHelper.isStoryDecopmosed(issue)}"/>
+    <s v="$[IF(AP2=&quot;Yes&quot;, N2, IF(AP2=&quot;No&quot;,0,&quot;&quot;))]"/>
+    <s v="$[IF(E2=&quot;Story: Done&quot;,0,IF(OR(B2=&quot;Story&quot;,B2=&quot;Spike&quot;), N2, &quot;&quot;))]&lt;/jt:forEach&gt;"/>
   </r>
   <r>
     <s v="&lt;jt:forEach items=&quot;${issues.subList(0, 0)}&quot; var=&quot;issue&quot; where=&quot;${issue.key = ''}&quot;&gt;"/>
@@ -1731,6 +1774,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -1774,6 +1820,9 @@
     <x v="2"/>
     <x v="2"/>
     <s v="POC"/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -1817,6 +1866,9 @@
     <x v="2"/>
     <x v="2"/>
     <s v="PROD"/>
+    <s v="Yes"/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -1860,6 +1912,9 @@
     <x v="2"/>
     <x v="2"/>
     <m/>
+    <s v="No"/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -1903,6 +1958,9 @@
     <x v="2"/>
     <x v="3"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -1946,6 +2004,9 @@
     <x v="2"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -1989,6 +2050,9 @@
     <x v="2"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2032,6 +2096,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2075,6 +2142,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2118,6 +2188,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2161,6 +2234,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2204,6 +2280,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2247,6 +2326,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2290,6 +2372,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2333,6 +2418,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2376,6 +2464,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2419,6 +2510,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2462,6 +2556,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2505,6 +2602,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2548,6 +2648,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2591,6 +2694,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2634,6 +2740,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2677,6 +2786,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2720,6 +2832,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2763,6 +2878,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2806,6 +2924,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2849,6 +2970,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2892,6 +3016,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2935,6 +3062,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -2978,6 +3108,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3021,6 +3154,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3064,6 +3200,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3107,6 +3246,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3150,6 +3292,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3193,6 +3338,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3236,6 +3384,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3279,6 +3430,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3322,6 +3476,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3365,6 +3522,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3408,6 +3568,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3451,6 +3614,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3494,6 +3660,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3537,6 +3706,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3580,6 +3752,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3623,6 +3798,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3666,6 +3844,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3709,6 +3890,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3752,6 +3936,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3795,6 +3982,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3838,6 +4028,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3881,6 +4074,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3924,6 +4120,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -3967,6 +4166,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -4010,6 +4212,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -4053,6 +4258,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -4096,6 +4304,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -4139,6 +4350,9 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="key"/>
@@ -4181,6 +4395,9 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
     <s v="&lt;/jt:forEach&gt;"/>
   </r>
   <r>
@@ -4224,15 +4441,18 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
     <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
+  <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
@@ -4373,8 +4593,13 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
@@ -4419,25 +4644,90 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
         <item h="1" x="0"/>
         <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
         <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item h="1" x="22"/>
+        <item h="1" x="15"/>
+        <item h="1" x="18"/>
+        <item h="1" x="16"/>
+        <item h="1" x="13"/>
+        <item h="1" x="17"/>
+        <item h="1" x="10"/>
+        <item h="1" x="19"/>
+        <item h="1" x="12"/>
+        <item h="1" x="20"/>
+        <item h="1" x="11"/>
+        <item h="1" x="14"/>
+        <item h="1" x="21"/>
+        <item h="1" x="35"/>
+        <item h="1" x="28"/>
+        <item h="1" x="31"/>
+        <item h="1" x="29"/>
+        <item h="1" x="26"/>
+        <item h="1" x="30"/>
+        <item h="1" x="23"/>
+        <item h="1" x="32"/>
+        <item h="1" x="25"/>
+        <item h="1" x="33"/>
+        <item h="1" x="24"/>
+        <item h="1" x="27"/>
+        <item h="1" x="34"/>
+        <item h="1" x="1"/>
+        <item h="1" x="46"/>
+        <item h="1" x="47"/>
+        <item h="1" x="48"/>
+        <item h="1" x="49"/>
+        <item h="1" x="50"/>
+        <item h="1" x="51"/>
+        <item h="1" x="52"/>
+        <item h="1" x="53"/>
+        <item h="1" x="54"/>
+        <item h="1" x="55"/>
+        <item h="1" x="56"/>
+        <item h="1" x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -4447,15 +4737,13 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -4474,19 +4762,19 @@
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+    <pivotField axis="axisRow" sortType="ascending">
       <items count="6">
-        <item x="0"/>
-        <item x="4"/>
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
       <items count="4">
         <item x="0"/>
@@ -4495,26 +4783,27 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="33"/>
   </rowFields>
-  <rowItems count="2">
+  <rowItems count="3">
     <i>
       <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -4524,36 +4813,23 @@
     <field x="1"/>
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="2">
     <i>
-      <x v="4"/>
+      <x v="2"/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
     </i>
-    <i>
-      <x v="5"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
   </colItems>
   <pageFields count="3">
     <pageField fld="30" hier="-1"/>
-    <pageField fld="38" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
     <pageField fld="37" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="2">
-    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
-    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="3" baseItem="4"/>
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="3" baseItem="4"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -4568,9 +4844,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -4686,6 +4962,7 @@
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" sortType="ascending"/>
     <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
       <items count="6">
         <item h="1" x="0"/>
@@ -4696,7 +4973,6 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
@@ -4710,12 +4986,17 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="33"/>
+    <field x="34"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -4757,9 +5038,163 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="38" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
+    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -4847,6 +5282,200 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item h="1" x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item h="1" x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item h="1" x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item h="1" x="1"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item h="1" x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -4899,7 +5528,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
@@ -4951,10 +5585,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
+  <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -5094,6 +5728,11 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -5146,394 +5785,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item h="1" x="22"/>
-        <item h="1" x="15"/>
-        <item h="1" x="18"/>
-        <item h="1" x="16"/>
-        <item h="1" x="13"/>
-        <item h="1" x="17"/>
-        <item h="1" x="10"/>
-        <item h="1" x="19"/>
-        <item h="1" x="12"/>
-        <item h="1" x="20"/>
-        <item h="1" x="11"/>
-        <item h="1" x="14"/>
-        <item h="1" x="21"/>
-        <item h="1" x="35"/>
-        <item h="1" x="28"/>
-        <item h="1" x="31"/>
-        <item h="1" x="29"/>
-        <item h="1" x="26"/>
-        <item h="1" x="30"/>
-        <item h="1" x="23"/>
-        <item h="1" x="32"/>
-        <item h="1" x="25"/>
-        <item h="1" x="33"/>
-        <item h="1" x="24"/>
-        <item h="1" x="27"/>
-        <item h="1" x="34"/>
-        <item h="1" x="1"/>
-        <item h="1" x="46"/>
-        <item h="1" x="47"/>
-        <item h="1" x="48"/>
-        <item h="1" x="49"/>
-        <item h="1" x="50"/>
-        <item h="1" x="51"/>
-        <item h="1" x="52"/>
-        <item h="1" x="53"/>
-        <item h="1" x="54"/>
-        <item h="1" x="55"/>
-        <item h="1" x="56"/>
-        <item h="1" x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="3" baseItem="4"/>
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="3" baseItem="4"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="44">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item h="1" x="16"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item h="1" x="35"/>
-        <item x="28"/>
-        <item x="31"/>
-        <item h="1" x="29"/>
-        <item x="26"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="27"/>
-        <item x="34"/>
-        <item h="1" x="1"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item h="1" x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" sortType="ascending"/>
-    <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="34"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
   <location ref="A7:H11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="44">
+  <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -5631,9 +5886,14 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="10"/>
@@ -5686,12 +5946,12 @@
     <dataField name="Story Estimate_x000a_(incl. Tech Debt &amp; Spikes)" fld="14" baseField="10" baseItem="1"/>
     <dataField name="Decomposed _x000a_(Ready, In Dev, Closed)" fld="22" baseField="10" baseItem="1"/>
     <dataField name="Remaining Estimate_x000a_(Not Closed/ Not Decomposed)" fld="16" baseField="10" baseItem="1"/>
-    <dataField name="Epic Decomposition Progress" fld="43" baseField="10" baseItem="0" numFmtId="9"/>
-    <dataField name="Story Decomposition Progress" fld="42" subtotal="count" baseField="10" baseItem="0"/>
-    <dataField name="Development Progress" fld="41" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
+    <dataField name="Epic Decomposition Progress" fld="46" baseField="10" baseItem="0" numFmtId="9"/>
+    <dataField name="Story Decomposition Progress" fld="45" subtotal="count" baseField="10" baseItem="0"/>
+    <dataField name="Development Progress" fld="44" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="19">
+    <format dxfId="15">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5701,7 +5961,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5711,7 +5971,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5721,7 +5981,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5731,10 +5991,263 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="11">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField name="To" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="60">
+        <item x="0"/>
+        <item x="41"/>
+        <item x="39"/>
+        <item x="43"/>
+        <item x="45"/>
+        <item x="36"/>
+        <item x="42"/>
+        <item x="38"/>
+        <item x="37"/>
+        <item x="40"/>
+        <item x="44"/>
+        <item x="58"/>
+        <item x="51"/>
+        <item x="54"/>
+        <item x="52"/>
+        <item x="49"/>
+        <item x="53"/>
+        <item x="46"/>
+        <item x="55"/>
+        <item x="48"/>
+        <item x="56"/>
+        <item x="47"/>
+        <item x="50"/>
+        <item x="57"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="10"/>
+    <field x="2"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+    <pageField fld="30" item="1" hier="-1"/>
+    <pageField fld="39" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Total Estimate" fld="13" baseField="10" baseItem="1"/>
+    <dataField name="Decomposed (Ready, In Dev, Closed) " fld="42" baseField="10" baseItem="1"/>
+    <dataField name="Remaining Estimate (Not Closed/Not Decomposed)" fld="43" baseField="10" baseItem="1"/>
+    <dataField name="Decomposition Progress" fld="47" baseField="0" baseItem="0" numFmtId="9"/>
+    <dataField name="Development Progress" fld="48" baseField="0" baseItem="0" numFmtId="9"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="3"/>
             <x v="4"/>
           </reference>
         </references>
@@ -6145,9 +6658,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -6212,18 +6725,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.21875" customWidth="1"/>
     <col min="14" max="14" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -6690,20 +7203,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -6844,9 +7357,148 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522E1814-F5A3-4A27-BA38-887B96B654B2}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="17">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="20">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="20">
+        <v>5</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="20">
+        <v>5</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="20">
+        <v>5</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:AP61"/>
+  <dimension ref="A1:AS61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6892,11 +7544,13 @@
     <col min="36" max="36" width="19.88671875" style="5" customWidth="1"/>
     <col min="37" max="37" width="18.77734375" style="5" customWidth="1"/>
     <col min="38" max="40" width="15.21875" style="5" customWidth="1"/>
-    <col min="41" max="41" width="17.5546875" style="5" customWidth="1"/>
-    <col min="42" max="16384" width="9.109375" style="3"/>
+    <col min="41" max="42" width="17.5546875" style="5" customWidth="1"/>
+    <col min="43" max="43" width="19.5546875" style="5" customWidth="1"/>
+    <col min="44" max="44" width="17.5546875" style="5" customWidth="1"/>
+    <col min="45" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -7020,11 +7674,20 @@
       <c r="AO1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="5" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="5" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
@@ -7146,18 +7809,27 @@
         <v>194</v>
       </c>
       <c r="AO2" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="AP2" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="AR2" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AS2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
@@ -7194,10 +7866,10 @@
         <v>11.4</v>
       </c>
       <c r="AO4" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" ht="27.6" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -7239,10 +7911,13 @@
         <v>11.4</v>
       </c>
       <c r="AO5" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="AP5" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -7284,8 +7959,11 @@
       <c r="AN6" s="5">
         <v>11.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AP6" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -7325,7 +8003,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -7356,7 +8034,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -7385,7 +8063,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>53</v>
       </c>
@@ -7411,7 +8089,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
@@ -7437,7 +8115,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
@@ -7463,7 +8141,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -7489,7 +8167,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
@@ -7511,7 +8189,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
@@ -7533,7 +8211,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>53</v>
       </c>
@@ -7900,7 +8578,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>53</v>
       </c>
@@ -7912,7 +8590,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>53</v>
       </c>
@@ -7924,7 +8602,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:41" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>53</v>
       </c>
@@ -7936,7 +8614,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>53</v>
       </c>
@@ -7948,7 +8626,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:41" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>53</v>
       </c>
@@ -7960,7 +8638,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>53</v>
       </c>
@@ -7972,7 +8650,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:41" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:44" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -7984,7 +8662,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:41" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:44" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -7996,7 +8674,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:41" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -8008,7 +8686,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:41" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -8019,7 +8697,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:41" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -8030,18 +8708,18 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="AO60" s="5" t="s">
+      <c r="AR60" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A61" s="31" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Fixed from blueprint-xray-planning-helper.groovy to blueprint-austin-planning-helper.groovy
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Austin-Issues.xlsx
+++ b/blueprint-jira-better-excel/Austin-Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3FDC45-C6EA-4DE1-82A7-5F16764C3F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D133DC-09CC-4945-A9A5-5528C3BA7028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="688" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="224" r:id="rId7"/>
+    <pivotCache cacheId="199" r:id="rId7"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1041,9 +1041,6 @@
     <t>X-Ray</t>
   </si>
   <si>
-    <t>&lt;mt:execute script="field-helper-tool.groovy"/&gt;&lt;mt:execute script="blueprint-helper.groovy"/&gt;&lt;mt:execute script="blueprint-xray-planning-helper.groovy"/&gt;</t>
-  </si>
-  <si>
     <t>Austin</t>
   </si>
   <si>
@@ -1102,6 +1099,9 @@
   </si>
   <si>
     <t xml:space="preserve">Decomposed (Ready, In Dev, Closed) </t>
+  </si>
+  <si>
+    <t>&lt;mt:execute script="field-helper-tool.groovy"/&gt;&lt;mt:execute script="blueprint-helper.groovy"/&gt;&lt;mt:execute script="blueprint-austin-planning-helper.groovy"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1348,34 +1348,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -1422,7 +1395,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44123.650799305557" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44124.764428935188" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -4450,7 +4423,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -4644,7 +4617,601 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item h="1" x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item h="1" x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item h="1" x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item h="1" x="1"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item h="1" x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item h="1" x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item h="1" x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item h="1" x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item h="1" x="1"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item h="1" x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Story Points" fld="13" baseField="3" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="14"/>
+        <item h="1" x="15"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item h="1" x="18"/>
+        <item h="1" x="19"/>
+        <item h="1" x="20"/>
+        <item h="1" x="21"/>
+        <item h="1" x="22"/>
+        <item h="1" x="23"/>
+        <item h="1" x="24"/>
+        <item h="1" x="25"/>
+        <item h="1" x="26"/>
+        <item h="1" x="27"/>
+        <item h="1" x="28"/>
+        <item h="1" x="29"/>
+        <item h="1" x="30"/>
+        <item h="1" x="31"/>
+        <item h="1" x="32"/>
+        <item h="1" x="33"/>
+        <item h="1" x="34"/>
+        <item h="1" x="35"/>
+        <item h="1" x="36"/>
+        <item h="1" x="37"/>
+        <item h="1" x="38"/>
+        <item h="1" x="39"/>
+        <item h="1" x="40"/>
+        <item h="1" x="41"/>
+        <item h="1" x="42"/>
+        <item h="1" x="43"/>
+        <item h="1" x="44"/>
+        <item h="1" x="45"/>
+        <item h="1" x="46"/>
+        <item h="1" x="47"/>
+        <item h="1" x="48"/>
+        <item h="1" x="49"/>
+        <item h="1" x="50"/>
+        <item h="1" x="51"/>
+        <item h="1" x="52"/>
+        <item h="1" x="53"/>
+        <item h="1" x="54"/>
+        <item h="1" x="55"/>
+        <item h="1" x="56"/>
+        <item h="1" x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i>
+      <x v="2"/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Estimate in Days" fld="12" baseField="3" baseItem="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -4843,8 +5410,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5037,8 +5604,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5191,602 +5758,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item h="1" x="16"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item h="1" x="35"/>
-        <item x="28"/>
-        <item x="31"/>
-        <item h="1" x="29"/>
-        <item x="26"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="27"/>
-        <item x="34"/>
-        <item h="1" x="1"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item h="1" x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item h="1" x="16"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item h="1" x="35"/>
-        <item x="28"/>
-        <item x="31"/>
-        <item h="1" x="29"/>
-        <item x="26"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="27"/>
-        <item x="34"/>
-        <item h="1" x="1"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item h="1" x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Story Points" fld="13" baseField="3" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item h="1" x="12"/>
-        <item h="1" x="13"/>
-        <item h="1" x="14"/>
-        <item h="1" x="15"/>
-        <item h="1" x="16"/>
-        <item h="1" x="17"/>
-        <item h="1" x="18"/>
-        <item h="1" x="19"/>
-        <item h="1" x="20"/>
-        <item h="1" x="21"/>
-        <item h="1" x="22"/>
-        <item h="1" x="23"/>
-        <item h="1" x="24"/>
-        <item h="1" x="25"/>
-        <item h="1" x="26"/>
-        <item h="1" x="27"/>
-        <item h="1" x="28"/>
-        <item h="1" x="29"/>
-        <item h="1" x="30"/>
-        <item h="1" x="31"/>
-        <item h="1" x="32"/>
-        <item h="1" x="33"/>
-        <item h="1" x="34"/>
-        <item h="1" x="35"/>
-        <item h="1" x="36"/>
-        <item h="1" x="37"/>
-        <item h="1" x="38"/>
-        <item h="1" x="39"/>
-        <item h="1" x="40"/>
-        <item h="1" x="41"/>
-        <item h="1" x="42"/>
-        <item h="1" x="43"/>
-        <item h="1" x="44"/>
-        <item h="1" x="45"/>
-        <item h="1" x="46"/>
-        <item h="1" x="47"/>
-        <item h="1" x="48"/>
-        <item h="1" x="49"/>
-        <item h="1" x="50"/>
-        <item h="1" x="51"/>
-        <item h="1" x="52"/>
-        <item h="1" x="53"/>
-        <item h="1" x="54"/>
-        <item h="1" x="55"/>
-        <item h="1" x="56"/>
-        <item h="1" x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i>
-      <x v="2"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Estimate in Days" fld="12" baseField="3" baseItem="4"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
   <location ref="A7:H11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5951,7 +5924,7 @@
     <dataField name="Development Progress" fld="44" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="15">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5961,7 +5934,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5971,7 +5944,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5981,7 +5954,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5991,7 +5964,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="2">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6014,7 +5987,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="224" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField showAll="0"/>
@@ -6230,7 +6203,7 @@
     <dataField name="Development Progress" fld="48" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="10">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -6243,7 +6216,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -6675,7 +6648,7 @@
         <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -6688,7 +6661,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="17">
         <v>11.3</v>
@@ -6725,11 +6698,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -6767,19 +6740,19 @@
         <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -6971,7 +6944,7 @@
         <v>148</v>
       </c>
       <c r="B22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -7089,13 +7062,13 @@
         <v>148</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>148</v>
       </c>
       <c r="H39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -7232,7 +7205,7 @@
         <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -7253,7 +7226,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" s="17">
         <v>11.4</v>
@@ -7366,17 +7339,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
         <v>65</v>
@@ -7395,12 +7368,12 @@
         <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="17">
         <v>11.4</v>
@@ -7408,19 +7381,19 @@
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>190</v>
@@ -7669,22 +7642,22 @@
         <v>153</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="AP1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AQ1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="AS1" s="3" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:45" s="5" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -7803,22 +7776,22 @@
         <v>179</v>
       </c>
       <c r="AM2" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AN2" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AO2" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AP2" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AR2" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="AR2" s="15" t="s">
-        <v>207</v>
       </c>
       <c r="AS2" s="5" t="s">
         <v>11</v>
@@ -7847,7 +7820,7 @@
       </c>
       <c r="W4" s="4"/>
       <c r="AE4" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH4" s="4" t="s">
         <v>158</v>
@@ -7866,7 +7839,7 @@
         <v>11.4</v>
       </c>
       <c r="AO4" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
@@ -7892,7 +7865,7 @@
       </c>
       <c r="W5" s="4"/>
       <c r="AE5" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH5" s="4" t="s">
         <v>158</v>
@@ -7911,7 +7884,7 @@
         <v>11.4</v>
       </c>
       <c r="AO5" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AP5" s="5" t="s">
         <v>155</v>
@@ -7960,7 +7933,7 @@
         <v>11.4</v>
       </c>
       <c r="AP6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.3">
@@ -7984,7 +7957,7 @@
       </c>
       <c r="W7" s="4"/>
       <c r="AE7" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH7" s="4" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Added the conditional formatting for Total Estimate equal to zero.
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Austin-Issues.xlsx
+++ b/blueprint-jira-better-excel/Austin-Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D133DC-09CC-4945-A9A5-5528C3BA7028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A018222B-829D-48B3-8B2D-B81CAB074567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="688" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="199" r:id="rId7"/>
+    <pivotCache cacheId="15" r:id="rId7"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1348,7 +1348,37 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -1395,7 +1425,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44124.764428935188" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44125.350823148146" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -1643,11 +1673,11 @@
     <cacheField name="Story Remaining SP" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Component Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Epic Remaining Estimate')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
-    <cacheField name="Component Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Epic Decomposed')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
-    <cacheField name="Component Epic Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Stories Estimate')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
-    <cacheField name="Story Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Story Decomposed SP')/SUM('Story Points'),1)" databaseField="0"/>
-    <cacheField name="Story Development Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Story Remaining SP')/SUM('Story Points'),1)" databaseField="0"/>
+    <cacheField name="Component Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Epic Remaining Estimate')/SUM('Epic Total Estimate'),0)" databaseField="0"/>
+    <cacheField name="Component Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Epic Decomposed')/SUM('Epic Total Estimate'),0)" databaseField="0"/>
+    <cacheField name="Component Epic Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Stories Estimate')/SUM('Epic Total Estimate'),0)" databaseField="0"/>
+    <cacheField name="Story Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Story Decomposed SP')/SUM('Story Points'),0)" databaseField="0"/>
+    <cacheField name="Story Development Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Story Remaining SP')/SUM('Story Points'),0)" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -4423,7 +4453,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -4617,8 +4647,208 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item h="1" x="22"/>
+        <item h="1" x="15"/>
+        <item h="1" x="18"/>
+        <item h="1" x="16"/>
+        <item h="1" x="13"/>
+        <item h="1" x="17"/>
+        <item h="1" x="10"/>
+        <item h="1" x="19"/>
+        <item h="1" x="12"/>
+        <item h="1" x="20"/>
+        <item h="1" x="11"/>
+        <item h="1" x="14"/>
+        <item h="1" x="21"/>
+        <item h="1" x="35"/>
+        <item h="1" x="28"/>
+        <item h="1" x="31"/>
+        <item h="1" x="29"/>
+        <item h="1" x="26"/>
+        <item h="1" x="30"/>
+        <item h="1" x="23"/>
+        <item h="1" x="32"/>
+        <item h="1" x="25"/>
+        <item h="1" x="33"/>
+        <item h="1" x="24"/>
+        <item h="1" x="27"/>
+        <item h="1" x="34"/>
+        <item h="1" x="1"/>
+        <item h="1" x="46"/>
+        <item h="1" x="47"/>
+        <item h="1" x="48"/>
+        <item h="1" x="49"/>
+        <item h="1" x="50"/>
+        <item h="1" x="51"/>
+        <item h="1" x="52"/>
+        <item h="1" x="53"/>
+        <item h="1" x="54"/>
+        <item h="1" x="55"/>
+        <item h="1" x="56"/>
+        <item h="1" x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="3" baseItem="4"/>
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="3" baseItem="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
@@ -4735,6 +4965,7 @@
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" sortType="ascending"/>
     <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
       <items count="6">
         <item h="1" x="0"/>
@@ -4745,7 +4976,6 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
@@ -4769,7 +4999,7 @@
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="33"/>
+    <field x="34"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -4810,9 +5040,163 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="38" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
+    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
@@ -4901,6 +5285,200 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item h="1" x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item h="1" x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item h="1" x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item h="1" x="1"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item h="1" x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5010,8 +5588,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5210,556 +5788,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item h="1" x="22"/>
-        <item h="1" x="15"/>
-        <item h="1" x="18"/>
-        <item h="1" x="16"/>
-        <item h="1" x="13"/>
-        <item h="1" x="17"/>
-        <item h="1" x="10"/>
-        <item h="1" x="19"/>
-        <item h="1" x="12"/>
-        <item h="1" x="20"/>
-        <item h="1" x="11"/>
-        <item h="1" x="14"/>
-        <item h="1" x="21"/>
-        <item h="1" x="35"/>
-        <item h="1" x="28"/>
-        <item h="1" x="31"/>
-        <item h="1" x="29"/>
-        <item h="1" x="26"/>
-        <item h="1" x="30"/>
-        <item h="1" x="23"/>
-        <item h="1" x="32"/>
-        <item h="1" x="25"/>
-        <item h="1" x="33"/>
-        <item h="1" x="24"/>
-        <item h="1" x="27"/>
-        <item h="1" x="34"/>
-        <item h="1" x="1"/>
-        <item h="1" x="46"/>
-        <item h="1" x="47"/>
-        <item h="1" x="48"/>
-        <item h="1" x="49"/>
-        <item h="1" x="50"/>
-        <item h="1" x="51"/>
-        <item h="1" x="52"/>
-        <item h="1" x="53"/>
-        <item h="1" x="54"/>
-        <item h="1" x="55"/>
-        <item h="1" x="56"/>
-        <item h="1" x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="3" baseItem="4"/>
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="3" baseItem="4"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item h="1" x="16"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item h="1" x="35"/>
-        <item x="28"/>
-        <item x="31"/>
-        <item h="1" x="29"/>
-        <item x="26"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="27"/>
-        <item x="34"/>
-        <item h="1" x="1"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item h="1" x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" sortType="ascending"/>
-    <pivotField axis="axisRow" subtotalTop="0" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="34"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x v="4"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="38" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
-    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
   <location ref="A7:H11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5924,7 +5954,7 @@
     <dataField name="Development Progress" fld="44" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="6">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5934,7 +5964,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5944,7 +5974,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5954,7 +5984,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5964,7 +5994,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -5987,7 +6017,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="199" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField showAll="0"/>
@@ -6203,7 +6233,7 @@
     <dataField name="Development Progress" fld="48" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -6216,7 +6246,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -6227,6 +6257,32 @@
       </pivotArea>
     </format>
   </formats>
+  <conditionalFormats count="2">
+    <conditionalFormat scope="field" priority="2">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="field" priority="1">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="10" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -6631,9 +6687,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -6698,18 +6754,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.21875" customWidth="1"/>
     <col min="14" max="14" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -7182,14 +7238,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -7285,13 +7341,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -7311,13 +7367,13 @@
         <v>0</v>
       </c>
       <c r="F11" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7339,10 +7395,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -7464,6 +7520,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting pivot="1" sqref="B8">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="B7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
The latest for Austin.
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Austin-Issues.xlsx
+++ b/blueprint-jira-better-excel/Austin-Issues.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A018222B-829D-48B3-8B2D-B81CAB074567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675D318F-4804-43F8-87FD-A2A6EEB71A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
     <sheet name="Bugs" sheetId="5" r:id="rId2"/>
     <sheet name="Development" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="Features (Epics)" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="Features (Stories)" sheetId="7" r:id="rId5"/>
-    <sheet name="Issues" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Components (Stories)" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="Features (Stories)" sheetId="8" r:id="rId6"/>
+    <sheet name="Issues" sheetId="2" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Issues!$A$1:$AS$61</definedName>
-    <definedName name="issues">OFFSET(Issues!$A$1,0,0,COUNTA(Issues!$A$1:$A$9999),COUNTA(Issues!$A$1:$AAO$1)-1)</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Issues!$A$1:$AT$61</definedName>
+    <definedName name="issues">OFFSET(Issues!$A$1,0,0,COUNTA(Issues!$A$1:$A$9999),COUNTA(Issues!$A$1:$AAP$1)-1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId7"/>
+    <pivotCache cacheId="28" r:id="rId8"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="225">
   <si>
     <t>Status</t>
   </si>
@@ -1044,12 +1045,6 @@
     <t>Austin</t>
   </si>
   <si>
-    <t>${fieldHelper.getFieldValueByName(issue, "Release #")}</t>
-  </si>
-  <si>
-    <t>Release #</t>
-  </si>
-  <si>
     <t>Quality Score</t>
   </si>
   <si>
@@ -1083,9 +1078,6 @@
     <t>$[IF(AP2="Yes", N2, IF(AP2="No",0,""))]</t>
   </si>
   <si>
-    <t>$[IF(E2="Story: Done",0,IF(OR(B2="Story",B2="Spike"), N2, ""))]&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -1102,14 +1094,60 @@
   </si>
   <si>
     <t>&lt;mt:execute script="field-helper-tool.groovy"/&gt;&lt;mt:execute script="blueprint-helper.groovy"/&gt;&lt;mt:execute script="blueprint-austin-planning-helper.groovy"/&gt;</t>
+  </si>
+  <si>
+    <t>Release Component</t>
+  </si>
+  <si>
+    <t>$[IF(E2="Story: Done",0,IF(OR(B2="Story",B2="Spike"), N2, ""))]</t>
+  </si>
+  <si>
+    <t>${bpHelper.getAustinComponent(issue)}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>AA Migration Demo PoC</t>
+  </si>
+  <si>
+    <t>Digital Blueprint Licensing</t>
+  </si>
+  <si>
+    <t>New Impact Analysis</t>
+  </si>
+  <si>
+    <t>Import/Export Projects MVP</t>
+  </si>
+  <si>
+    <t>AD and FA Settings</t>
+  </si>
+  <si>
+    <t>Convert Custom Properties to Standard</t>
+  </si>
+  <si>
+    <t>Pre-Loaded Instance Configuration</t>
+  </si>
+  <si>
+    <t>Dropping SQL Server 2012</t>
+  </si>
+  <si>
+    <t>R&amp;D Bucket</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Active in Release #</t>
+  </si>
+  <si>
+    <t>${fieldHelper.getFieldValueByName(issue, "Active in Release #")}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1251,7 +1289,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1342,13 +1380,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="23">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1358,6 +1438,12 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <font>
@@ -1378,12 +1464,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -1425,11 +1505,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44125.350823148146" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="44180.643165624999" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
-  <cacheFields count="49">
+  <cacheFields count="50">
     <cacheField name="Key" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -1653,10 +1733,11 @@
         <s v="Yes"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Release #" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="11.3" maxValue="11.4" count="4">
-        <s v="${fieldHelper.getFieldValueByName(issue, &quot;Release #&quot;)}"/>
+    <cacheField name="Active in Release #" numFmtId="0">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="11.3" maxValue="12" count="5">
+        <s v="${fieldHelper.getFieldValueByName(issue, &quot;Active in Release #&quot;)}"/>
         <m/>
+        <n v="12"/>
         <n v="11.4"/>
         <n v="11.3"/>
       </sharedItems>
@@ -1672,6 +1753,23 @@
     </cacheField>
     <cacheField name="Story Remaining SP" numFmtId="0">
       <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Release Component" numFmtId="0">
+      <sharedItems containsBlank="1" count="13">
+        <s v="${bpHelper.getAustinComponent(issue)}&lt;/jt:forEach&gt;"/>
+        <m/>
+        <s v="AA Migration Demo PoC"/>
+        <s v="Digital Blueprint Licensing"/>
+        <s v="New Impact Analysis"/>
+        <s v="Import/Export Projects MVP"/>
+        <s v="AD and FA Settings"/>
+        <s v="Convert Custom Properties to Standard"/>
+        <s v="Pre-Loaded Instance Configuration"/>
+        <s v="Dropping SQL Server 2012"/>
+        <s v="R&amp;D Bucket"/>
+        <s v="Other"/>
+        <s v="&lt;/jt:forEach&gt;"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Component Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Epic Remaining Estimate')/SUM('Epic Total Estimate'),0)" databaseField="0"/>
     <cacheField name="Component Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Epic Decomposed')/SUM('Epic Total Estimate'),0)" databaseField="0"/>
@@ -1733,7 +1831,8 @@
     <s v="${fieldHelper.getFieldValueByName(issue, &quot;Quality Score&quot;)}"/>
     <s v="${bpHelper.isStoryDecopmosed(issue)}"/>
     <s v="$[IF(AP2=&quot;Yes&quot;, N2, IF(AP2=&quot;No&quot;,0,&quot;&quot;))]"/>
-    <s v="$[IF(E2=&quot;Story: Done&quot;,0,IF(OR(B2=&quot;Story&quot;,B2=&quot;Spike&quot;), N2, &quot;&quot;))]&lt;/jt:forEach&gt;"/>
+    <s v="$[IF(E2=&quot;Story: Done&quot;,0,IF(OR(B2=&quot;Story&quot;,B2=&quot;Spike&quot;), N2, &quot;&quot;))]"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="&lt;jt:forEach items=&quot;${issues.subList(0, 0)}&quot; var=&quot;issue&quot; where=&quot;${issue.key = ''}&quot;&gt;"/>
@@ -1780,6 +1879,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -1826,6 +1926,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -1872,6 +1973,7 @@
     <s v="Yes"/>
     <m/>
     <m/>
+    <x v="3"/>
   </r>
   <r>
     <s v="key"/>
@@ -1918,6 +2020,7 @@
     <s v="No"/>
     <m/>
     <m/>
+    <x v="4"/>
   </r>
   <r>
     <s v="key"/>
@@ -1964,6 +2067,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="5"/>
   </r>
   <r>
     <s v="key"/>
@@ -2005,11 +2109,12 @@
     <m/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <x v="4"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="6"/>
   </r>
   <r>
     <s v="key"/>
@@ -2056,6 +2161,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="7"/>
   </r>
   <r>
     <s v="key"/>
@@ -2102,6 +2208,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="8"/>
   </r>
   <r>
     <s v="key"/>
@@ -2148,6 +2255,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="9"/>
   </r>
   <r>
     <s v="key"/>
@@ -2194,6 +2302,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="10"/>
   </r>
   <r>
     <s v="key"/>
@@ -2240,6 +2349,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="11"/>
   </r>
   <r>
     <s v="key"/>
@@ -2286,6 +2396,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2332,6 +2443,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2378,6 +2490,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2424,6 +2537,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2470,6 +2584,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2516,6 +2631,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2562,6 +2678,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2608,6 +2725,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2654,6 +2772,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2700,6 +2819,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2746,6 +2866,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2792,6 +2913,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2838,6 +2960,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2884,6 +3007,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2930,6 +3054,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -2976,6 +3101,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3022,6 +3148,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3068,6 +3195,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3114,6 +3242,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3160,6 +3289,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3206,6 +3336,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3252,6 +3383,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3298,6 +3430,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3344,6 +3477,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3390,6 +3524,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3436,6 +3571,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3482,6 +3618,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3528,6 +3665,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3574,6 +3712,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3620,6 +3759,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3666,6 +3806,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3712,6 +3853,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3758,6 +3900,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3804,6 +3947,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3850,6 +3994,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3896,6 +4041,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3942,6 +4088,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -3988,6 +4135,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4034,6 +4182,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4080,6 +4229,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4126,6 +4276,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4172,6 +4323,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4218,6 +4370,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4264,6 +4417,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4310,6 +4464,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4356,6 +4511,7 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -4401,7 +4557,8 @@
     <m/>
     <m/>
     <m/>
-    <s v="&lt;/jt:forEach&gt;"/>
+    <m/>
+    <x v="12"/>
   </r>
   <r>
     <s v="key"/>
@@ -4448,14 +4605,15 @@
     <m/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A6:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
+  <pivotFields count="50">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
@@ -4587,14 +4745,16 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
-      <items count="5">
+      <items count="6">
+        <item x="4"/>
         <item x="3"/>
-        <item x="2"/>
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -4628,7 +4788,7 @@
   <pageFields count="3">
     <pageField fld="30" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="39" item="0" hier="-1"/>
+    <pageField fld="39" item="4" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Bug Count" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -4646,10 +4806,491 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{47FAF9B3-F1B1-4B18-B603-59ADFB7917AB}" name="PivotTable4" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="50">
+    <pivotField showAll="0"/>
+    <pivotField name="To" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="60">
+        <item x="0"/>
+        <item x="41"/>
+        <item x="39"/>
+        <item x="43"/>
+        <item x="45"/>
+        <item x="36"/>
+        <item x="42"/>
+        <item x="38"/>
+        <item x="37"/>
+        <item x="40"/>
+        <item x="44"/>
+        <item x="58"/>
+        <item x="51"/>
+        <item x="54"/>
+        <item x="52"/>
+        <item x="49"/>
+        <item x="53"/>
+        <item x="46"/>
+        <item x="55"/>
+        <item x="48"/>
+        <item x="56"/>
+        <item x="47"/>
+        <item x="50"/>
+        <item x="57"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" sortType="ascending"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="14">
+        <item x="0"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="44"/>
+    <field x="2"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+    <pageField fld="30" item="1" hier="-1"/>
+    <pageField fld="39" item="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Total Estimate" fld="13" baseField="10" baseItem="1"/>
+    <dataField name="Decomposed (Ready, In Dev, Closed) " fld="42" baseField="10" baseItem="1"/>
+    <dataField name="Remaining Estimate (Not Closed/Not Decomposed)" fld="43" baseField="10" baseItem="1"/>
+    <dataField name="Decomposition Progress" fld="48" baseField="0" baseItem="0" numFmtId="9"/>
+    <dataField name="Development Progress" fld="49" baseField="0" baseItem="0" numFmtId="9"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <conditionalFormats count="1">
+    <conditionalFormat scope="field" priority="2">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="50">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="60">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="14"/>
+        <item h="1" x="15"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item h="1" x="18"/>
+        <item h="1" x="19"/>
+        <item h="1" x="20"/>
+        <item h="1" x="21"/>
+        <item h="1" x="22"/>
+        <item h="1" x="23"/>
+        <item h="1" x="24"/>
+        <item h="1" x="25"/>
+        <item h="1" x="26"/>
+        <item h="1" x="27"/>
+        <item h="1" x="28"/>
+        <item h="1" x="29"/>
+        <item h="1" x="30"/>
+        <item h="1" x="31"/>
+        <item h="1" x="32"/>
+        <item h="1" x="33"/>
+        <item h="1" x="34"/>
+        <item h="1" x="35"/>
+        <item h="1" x="36"/>
+        <item h="1" x="37"/>
+        <item h="1" x="38"/>
+        <item h="1" x="39"/>
+        <item h="1" x="40"/>
+        <item h="1" x="41"/>
+        <item h="1" x="42"/>
+        <item h="1" x="43"/>
+        <item h="1" x="44"/>
+        <item h="1" x="45"/>
+        <item h="1" x="46"/>
+        <item h="1" x="47"/>
+        <item h="1" x="48"/>
+        <item h="1" x="49"/>
+        <item h="1" x="50"/>
+        <item h="1" x="51"/>
+        <item h="1" x="52"/>
+        <item h="1" x="53"/>
+        <item h="1" x="54"/>
+        <item h="1" x="55"/>
+        <item h="1" x="56"/>
+        <item h="1" x="57"/>
+        <item h="1" x="58"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" sortType="ascending">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i>
+      <x v="2"/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Estimate in Days" fld="12" baseField="3" baseItem="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="J6:L11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
+  <pivotFields count="50">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -4792,6 +5433,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -4846,10 +5488,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="G43:H47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
+  <pivotFields count="50">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -4992,6 +5634,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -5040,10 +5683,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A26:G30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
+  <pivotFields count="50">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -5125,6 +5768,7 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -5194,10 +5838,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A43:B47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
+  <pivotFields count="50">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -5340,6 +5984,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -5388,10 +6033,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="D6:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
+  <pivotFields count="50">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -5534,6 +6179,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -5588,210 +6234,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A6:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="60">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item h="1" x="12"/>
-        <item h="1" x="13"/>
-        <item h="1" x="14"/>
-        <item h="1" x="15"/>
-        <item h="1" x="16"/>
-        <item h="1" x="17"/>
-        <item h="1" x="18"/>
-        <item h="1" x="19"/>
-        <item h="1" x="20"/>
-        <item h="1" x="21"/>
-        <item h="1" x="22"/>
-        <item h="1" x="23"/>
-        <item h="1" x="24"/>
-        <item h="1" x="25"/>
-        <item h="1" x="26"/>
-        <item h="1" x="27"/>
-        <item h="1" x="28"/>
-        <item h="1" x="29"/>
-        <item h="1" x="30"/>
-        <item h="1" x="31"/>
-        <item h="1" x="32"/>
-        <item h="1" x="33"/>
-        <item h="1" x="34"/>
-        <item h="1" x="35"/>
-        <item h="1" x="36"/>
-        <item h="1" x="37"/>
-        <item h="1" x="38"/>
-        <item h="1" x="39"/>
-        <item h="1" x="40"/>
-        <item h="1" x="41"/>
-        <item h="1" x="42"/>
-        <item h="1" x="43"/>
-        <item h="1" x="44"/>
-        <item h="1" x="45"/>
-        <item h="1" x="46"/>
-        <item h="1" x="47"/>
-        <item h="1" x="48"/>
-        <item h="1" x="49"/>
-        <item h="1" x="50"/>
-        <item h="1" x="51"/>
-        <item h="1" x="52"/>
-        <item h="1" x="53"/>
-        <item h="1" x="54"/>
-        <item h="1" x="55"/>
-        <item h="1" x="56"/>
-        <item h="1" x="57"/>
-        <item h="1" x="58"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" sortType="ascending">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i>
-      <x v="2"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Estimate in Days" fld="12" baseField="3" baseItem="4"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
-  <location ref="A7:H11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="49">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+  <location ref="A7:H11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="50">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -5879,15 +6325,8 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -5938,23 +6377,22 @@
       <x v="6"/>
     </i>
   </colItems>
-  <pageFields count="4">
+  <pageFields count="3">
     <pageField fld="30" hier="-1"/>
     <pageField fld="3" hier="-1"/>
     <pageField fld="37" item="0" hier="-1"/>
-    <pageField fld="39" item="3" hier="-1"/>
   </pageFields>
   <dataFields count="7">
     <dataField name="Total Estimate" fld="15" baseField="10" baseItem="1"/>
     <dataField name="Story Estimate_x000a_(incl. Tech Debt &amp; Spikes)" fld="14" baseField="10" baseItem="1"/>
     <dataField name="Decomposed _x000a_(Ready, In Dev, Closed)" fld="22" baseField="10" baseItem="1"/>
     <dataField name="Remaining Estimate_x000a_(Not Closed/ Not Decomposed)" fld="16" baseField="10" baseItem="1"/>
-    <dataField name="Epic Decomposition Progress" fld="46" baseField="10" baseItem="0" numFmtId="9"/>
-    <dataField name="Story Decomposition Progress" fld="45" subtotal="count" baseField="10" baseItem="0"/>
-    <dataField name="Development Progress" fld="44" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
+    <dataField name="Epic Decomposition Progress" fld="47" baseField="10" baseItem="0" numFmtId="9"/>
+    <dataField name="Story Decomposition Progress" fld="46" subtotal="count" baseField="10" baseItem="0"/>
+    <dataField name="Development Progress" fld="45" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="9">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -5964,7 +6402,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5974,7 +6412,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5984,7 +6422,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1">
@@ -5994,7 +6432,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="18">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6017,9 +6455,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="49">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13C56903-1401-4E6A-9D9D-8FBAEA31413A}" name="PivotTable4" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A6:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="50">
     <pivotField showAll="0"/>
     <pivotField name="To" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
@@ -6161,19 +6599,12 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -6219,21 +6650,20 @@
       <x v="4"/>
     </i>
   </colItems>
-  <pageFields count="4">
+  <pageFields count="3">
     <pageField fld="1" hier="-1"/>
     <pageField fld="37" item="1" hier="-1"/>
     <pageField fld="30" item="1" hier="-1"/>
-    <pageField fld="39" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="5">
     <dataField name="Total Estimate" fld="13" baseField="10" baseItem="1"/>
     <dataField name="Decomposed (Ready, In Dev, Closed) " fld="42" baseField="10" baseItem="1"/>
     <dataField name="Remaining Estimate (Not Closed/Not Decomposed)" fld="43" baseField="10" baseItem="1"/>
-    <dataField name="Decomposition Progress" fld="47" baseField="0" baseItem="0" numFmtId="9"/>
-    <dataField name="Development Progress" fld="48" baseField="0" baseItem="0" numFmtId="9"/>
+    <dataField name="Decomposition Progress" fld="48" baseField="0" baseItem="0" numFmtId="9"/>
+    <dataField name="Development Progress" fld="49" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="4">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -6246,7 +6676,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="14">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -6258,6 +6688,18 @@
     </format>
   </formats>
   <conditionalFormats count="2">
+    <conditionalFormat scope="field" priority="1">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="10" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat scope="field" priority="2">
       <pivotAreas count="1">
         <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -6266,18 +6708,6 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="0" selected="0"/>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat scope="field" priority="1">
-      <pivotAreas count="1">
-        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="10" count="0" selected="0"/>
           </references>
         </pivotArea>
       </pivotAreas>
@@ -6683,11 +7113,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -6717,10 +7149,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="B4" s="17">
-        <v>11.3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6754,7 +7186,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -7256,36 +7688,28 @@
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>178</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="17">
-        <v>11.4</v>
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -7387,9 +7811,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522E1814-F5A3-4A27-BA38-887B96B654B2}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -7403,53 +7827,45 @@
     <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" s="17">
-        <v>11.4</v>
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>190</v>
@@ -7521,12 +7937,12 @@
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="B8">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="B7">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7535,9 +7951,153 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF66290E-43B2-4D8C-B12D-4C7A8A7BDD6A}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="20">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="20">
+        <v>5</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="20">
+        <v>5</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="20">
+        <v>5</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting pivot="1" sqref="B8">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:AS61"/>
+  <dimension ref="A1:AT206"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7582,14 +8142,16 @@
     <col min="35" max="35" width="18.88671875" style="5" customWidth="1"/>
     <col min="36" max="36" width="19.88671875" style="5" customWidth="1"/>
     <col min="37" max="37" width="18.77734375" style="5" customWidth="1"/>
-    <col min="38" max="40" width="15.21875" style="5" customWidth="1"/>
+    <col min="38" max="39" width="15.21875" style="5" customWidth="1"/>
+    <col min="40" max="40" width="19.109375" style="5" customWidth="1"/>
     <col min="41" max="42" width="17.5546875" style="5" customWidth="1"/>
     <col min="43" max="43" width="19.5546875" style="5" customWidth="1"/>
     <col min="44" max="44" width="17.5546875" style="5" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="3"/>
+    <col min="45" max="45" width="33.5546875" style="5" customWidth="1"/>
+    <col min="46" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -7708,25 +8270,28 @@
         <v>153</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" s="5" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" s="5" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
@@ -7842,33 +8407,37 @@
         <v>179</v>
       </c>
       <c r="AM2" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AN2" s="15" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="AO2" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AP2" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AQ2" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AR2" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="AS2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="AT2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN3" s="36"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
@@ -7901,14 +8470,17 @@
       <c r="AM4" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AN4" s="5">
-        <v>11.4</v>
+      <c r="AN4" s="36">
+        <v>12</v>
       </c>
       <c r="AO4" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="AS4" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -7946,17 +8518,20 @@
       <c r="AM5" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AN5" s="5">
-        <v>11.4</v>
+      <c r="AN5" s="36">
+        <v>12</v>
       </c>
       <c r="AO5" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AP5" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AS5" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -7995,14 +8570,17 @@
       <c r="AM6" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AN6" s="5">
-        <v>11.4</v>
+      <c r="AN6" s="36">
+        <v>12</v>
       </c>
       <c r="AP6" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="AS6" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -8038,11 +8616,14 @@
       <c r="AM7" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AN7" s="5">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN7" s="36">
+        <v>11.4</v>
+      </c>
+      <c r="AS7" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -8072,8 +8653,14 @@
       <c r="AM8" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN8" s="36">
+        <v>11.3</v>
+      </c>
+      <c r="AS8" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -8101,8 +8688,12 @@
       <c r="AM9" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN9" s="36"/>
+      <c r="AS9" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>53</v>
       </c>
@@ -8127,8 +8718,12 @@
       <c r="AL10" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN10" s="36"/>
+      <c r="AS10" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
@@ -8153,8 +8748,12 @@
       <c r="AL11" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN11" s="36"/>
+      <c r="AS11" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
@@ -8179,8 +8778,12 @@
       <c r="AL12" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN12" s="36"/>
+      <c r="AS12" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -8205,8 +8808,12 @@
       <c r="AL13" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN13" s="36"/>
+      <c r="AS13" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
@@ -8227,8 +8834,9 @@
       <c r="AL14" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN14" s="36"/>
+    </row>
+    <row r="15" spans="1:46" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
@@ -8249,8 +8857,9 @@
       <c r="AL15" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN15" s="36"/>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>53</v>
       </c>
@@ -8263,8 +8872,9 @@
       <c r="AL16" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN16" s="36"/>
+    </row>
+    <row r="17" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>53</v>
       </c>
@@ -8274,8 +8884,9 @@
       <c r="AL17" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN17" s="36"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -8285,8 +8896,9 @@
       <c r="AL18" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="19" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN18" s="36"/>
+    </row>
+    <row r="19" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>53</v>
       </c>
@@ -8296,8 +8908,9 @@
       <c r="AL19" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="20" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN19" s="36"/>
+    </row>
+    <row r="20" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>53</v>
       </c>
@@ -8307,8 +8920,9 @@
       <c r="AL20" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="21" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN20" s="36"/>
+    </row>
+    <row r="21" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -8318,8 +8932,9 @@
       <c r="AL21" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN21" s="36"/>
+    </row>
+    <row r="22" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>53</v>
       </c>
@@ -8329,8 +8944,9 @@
       <c r="AL22" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="23" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN22" s="36"/>
+    </row>
+    <row r="23" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
@@ -8340,8 +8956,9 @@
       <c r="AL23" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN23" s="36"/>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>53</v>
       </c>
@@ -8351,8 +8968,9 @@
       <c r="AL24" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN24" s="36"/>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
@@ -8362,8 +8980,9 @@
       <c r="AL25" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN25" s="36"/>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -8373,8 +8992,9 @@
       <c r="AL26" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN26" s="36"/>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>53</v>
       </c>
@@ -8384,8 +9004,9 @@
       <c r="AL27" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="28" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN27" s="36"/>
+    </row>
+    <row r="28" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
@@ -8395,8 +9016,9 @@
       <c r="AL28" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN28" s="36"/>
+    </row>
+    <row r="29" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>53</v>
       </c>
@@ -8406,8 +9028,9 @@
       <c r="AL29" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="30" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN29" s="36"/>
+    </row>
+    <row r="30" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -8417,8 +9040,9 @@
       <c r="AL30" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN30" s="36"/>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>53</v>
       </c>
@@ -8428,8 +9052,9 @@
       <c r="AL31" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN31" s="36"/>
+    </row>
+    <row r="32" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
@@ -8439,8 +9064,9 @@
       <c r="AL32" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN32" s="36"/>
+    </row>
+    <row r="33" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
@@ -8450,8 +9076,9 @@
       <c r="AL33" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN33" s="36"/>
+    </row>
+    <row r="34" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>53</v>
       </c>
@@ -8461,8 +9088,9 @@
       <c r="AL34" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="35" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN34" s="36"/>
+    </row>
+    <row r="35" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>53</v>
       </c>
@@ -8472,8 +9100,9 @@
       <c r="AL35" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="36" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN35" s="36"/>
+    </row>
+    <row r="36" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>53</v>
       </c>
@@ -8483,8 +9112,9 @@
       <c r="AL36" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="37" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN36" s="36"/>
+    </row>
+    <row r="37" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>53</v>
       </c>
@@ -8494,8 +9124,9 @@
       <c r="AL37" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN37" s="36"/>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>53</v>
       </c>
@@ -8505,8 +9136,9 @@
       <c r="AL38" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN38" s="36"/>
+    </row>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>53</v>
       </c>
@@ -8516,8 +9148,9 @@
       <c r="AL39" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN39" s="36"/>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>53</v>
       </c>
@@ -8527,8 +9160,9 @@
       <c r="AL40" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="41" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN40" s="36"/>
+    </row>
+    <row r="41" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>53</v>
       </c>
@@ -8538,8 +9172,9 @@
       <c r="AL41" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN41" s="36"/>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>53</v>
       </c>
@@ -8549,8 +9184,9 @@
       <c r="AL42" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN42" s="36"/>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>53</v>
       </c>
@@ -8560,8 +9196,9 @@
       <c r="AL43" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN43" s="36"/>
+    </row>
+    <row r="44" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>53</v>
       </c>
@@ -8571,8 +9208,9 @@
       <c r="AL44" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="45" spans="1:38" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN44" s="36"/>
+    </row>
+    <row r="45" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>53</v>
       </c>
@@ -8582,8 +9220,9 @@
       <c r="AL45" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="46" spans="1:38" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN45" s="36"/>
+    </row>
+    <row r="46" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>53</v>
       </c>
@@ -8593,8 +9232,9 @@
       <c r="AL46" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN46" s="36"/>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
@@ -8604,8 +9244,9 @@
       <c r="AL47" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN47" s="36"/>
+    </row>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>53</v>
       </c>
@@ -8616,8 +9257,9 @@
       <c r="AL48" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AN48" s="36"/>
+    </row>
+    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>53</v>
       </c>
@@ -8628,8 +9270,9 @@
       <c r="AL49" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AN49" s="36"/>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>53</v>
       </c>
@@ -8640,8 +9283,9 @@
       <c r="AL50" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="51" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN50" s="36"/>
+    </row>
+    <row r="51" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>53</v>
       </c>
@@ -8652,8 +9296,9 @@
       <c r="AL51" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AN51" s="36"/>
+    </row>
+    <row r="52" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>53</v>
       </c>
@@ -8664,8 +9309,9 @@
       <c r="AL52" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="53" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN52" s="36"/>
+    </row>
+    <row r="53" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>53</v>
       </c>
@@ -8676,8 +9322,9 @@
       <c r="AL53" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AN53" s="36"/>
+    </row>
+    <row r="54" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>53</v>
       </c>
@@ -8688,8 +9335,9 @@
       <c r="AL54" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="55" spans="1:44" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN54" s="36"/>
+    </row>
+    <row r="55" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -8700,8 +9348,9 @@
       <c r="AL55" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="56" spans="1:44" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="AN55" s="36"/>
+    </row>
+    <row r="56" spans="1:45" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -8712,8 +9361,9 @@
       <c r="AL56" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="57" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN56" s="36"/>
+    </row>
+    <row r="57" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -8724,8 +9374,9 @@
       <c r="AL57" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="58" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN57" s="36"/>
+    </row>
+    <row r="58" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -8735,8 +9386,9 @@
       <c r="AL58" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="59" spans="1:44" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="AN58" s="36"/>
+    </row>
+    <row r="59" spans="1:45" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -8746,25 +9398,463 @@
       <c r="AL59" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AN59" s="36"/>
+    </row>
+    <row r="60" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="AR60" s="5" t="s">
+      <c r="AN60" s="36"/>
+      <c r="AS60" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A61" s="31" t="s">
         <v>53</v>
       </c>
       <c r="AH61" s="32" t="s">
         <v>55</v>
       </c>
+      <c r="AN61" s="36"/>
+    </row>
+    <row r="62" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN62" s="36"/>
+    </row>
+    <row r="63" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN63" s="36"/>
+    </row>
+    <row r="64" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AN64" s="36"/>
+    </row>
+    <row r="65" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN65" s="36"/>
+    </row>
+    <row r="66" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN66" s="36"/>
+    </row>
+    <row r="67" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN67" s="36"/>
+    </row>
+    <row r="68" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN68" s="36"/>
+    </row>
+    <row r="69" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN69" s="36"/>
+    </row>
+    <row r="70" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN70" s="36"/>
+    </row>
+    <row r="71" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN71" s="36"/>
+    </row>
+    <row r="72" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN72" s="36"/>
+    </row>
+    <row r="73" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN73" s="36"/>
+    </row>
+    <row r="74" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN74" s="36"/>
+    </row>
+    <row r="75" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN75" s="36"/>
+    </row>
+    <row r="76" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN76" s="36"/>
+    </row>
+    <row r="77" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN77" s="36"/>
+    </row>
+    <row r="78" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN78" s="36"/>
+    </row>
+    <row r="79" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN79" s="36"/>
+    </row>
+    <row r="80" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN80" s="36"/>
+    </row>
+    <row r="81" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN81" s="36"/>
+    </row>
+    <row r="82" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN82" s="36"/>
+    </row>
+    <row r="83" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN83" s="36"/>
+    </row>
+    <row r="84" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN84" s="36"/>
+    </row>
+    <row r="85" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN85" s="36"/>
+    </row>
+    <row r="86" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN86" s="36"/>
+    </row>
+    <row r="87" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN87" s="36"/>
+    </row>
+    <row r="88" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN88" s="36"/>
+    </row>
+    <row r="89" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN89" s="36"/>
+    </row>
+    <row r="90" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN90" s="36"/>
+    </row>
+    <row r="91" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN91" s="36"/>
+    </row>
+    <row r="92" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN92" s="36"/>
+    </row>
+    <row r="93" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN93" s="36"/>
+    </row>
+    <row r="94" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN94" s="36"/>
+    </row>
+    <row r="95" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN95" s="36"/>
+    </row>
+    <row r="96" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN96" s="36"/>
+    </row>
+    <row r="97" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN97" s="36"/>
+    </row>
+    <row r="98" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN98" s="36"/>
+    </row>
+    <row r="99" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN99" s="36"/>
+    </row>
+    <row r="100" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN100" s="36"/>
+    </row>
+    <row r="101" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN101" s="36"/>
+    </row>
+    <row r="102" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN102" s="36"/>
+    </row>
+    <row r="103" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN103" s="36"/>
+    </row>
+    <row r="104" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN104" s="36"/>
+    </row>
+    <row r="105" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN105" s="36"/>
+    </row>
+    <row r="106" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN106" s="36"/>
+    </row>
+    <row r="107" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN107" s="36"/>
+    </row>
+    <row r="108" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN108" s="36"/>
+    </row>
+    <row r="109" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN109" s="36"/>
+    </row>
+    <row r="110" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN110" s="36"/>
+    </row>
+    <row r="111" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN111" s="36"/>
+    </row>
+    <row r="112" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN112" s="36"/>
+    </row>
+    <row r="113" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN113" s="36"/>
+    </row>
+    <row r="114" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN114" s="36"/>
+    </row>
+    <row r="115" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN115" s="36"/>
+    </row>
+    <row r="116" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN116" s="36"/>
+    </row>
+    <row r="117" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN117" s="36"/>
+    </row>
+    <row r="118" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN118" s="36"/>
+    </row>
+    <row r="119" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN119" s="36"/>
+    </row>
+    <row r="120" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN120" s="36"/>
+    </row>
+    <row r="121" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN121" s="36"/>
+    </row>
+    <row r="122" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN122" s="36"/>
+    </row>
+    <row r="123" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN123" s="36"/>
+    </row>
+    <row r="124" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN124" s="36"/>
+    </row>
+    <row r="125" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN125" s="36"/>
+    </row>
+    <row r="126" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN126" s="36"/>
+    </row>
+    <row r="127" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN127" s="36"/>
+    </row>
+    <row r="128" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN128" s="36"/>
+    </row>
+    <row r="129" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN129" s="36"/>
+    </row>
+    <row r="130" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN130" s="36"/>
+    </row>
+    <row r="131" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN131" s="36"/>
+    </row>
+    <row r="132" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN132" s="36"/>
+    </row>
+    <row r="133" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN133" s="36"/>
+    </row>
+    <row r="134" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN134" s="36"/>
+    </row>
+    <row r="135" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN135" s="36"/>
+    </row>
+    <row r="136" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN136" s="36"/>
+    </row>
+    <row r="137" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN137" s="36"/>
+    </row>
+    <row r="138" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN138" s="36"/>
+    </row>
+    <row r="139" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN139" s="36"/>
+    </row>
+    <row r="140" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN140" s="36"/>
+    </row>
+    <row r="141" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN141" s="36"/>
+    </row>
+    <row r="142" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN142" s="36"/>
+    </row>
+    <row r="143" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN143" s="36"/>
+    </row>
+    <row r="144" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN144" s="36"/>
+    </row>
+    <row r="145" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN145" s="36"/>
+    </row>
+    <row r="146" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN146" s="36"/>
+    </row>
+    <row r="147" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN147" s="36"/>
+    </row>
+    <row r="148" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN148" s="36"/>
+    </row>
+    <row r="149" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN149" s="36"/>
+    </row>
+    <row r="150" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN150" s="36"/>
+    </row>
+    <row r="151" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN151" s="36"/>
+    </row>
+    <row r="152" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN152" s="36"/>
+    </row>
+    <row r="153" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN153" s="36"/>
+    </row>
+    <row r="154" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN154" s="36"/>
+    </row>
+    <row r="155" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN155" s="36"/>
+    </row>
+    <row r="156" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN156" s="36"/>
+    </row>
+    <row r="157" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN157" s="36"/>
+    </row>
+    <row r="158" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN158" s="36"/>
+    </row>
+    <row r="159" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN159" s="36"/>
+    </row>
+    <row r="160" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN160" s="36"/>
+    </row>
+    <row r="161" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN161" s="36"/>
+    </row>
+    <row r="162" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN162" s="36"/>
+    </row>
+    <row r="163" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN163" s="36"/>
+    </row>
+    <row r="164" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN164" s="36"/>
+    </row>
+    <row r="165" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN165" s="36"/>
+    </row>
+    <row r="166" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN166" s="36"/>
+    </row>
+    <row r="167" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN167" s="36"/>
+    </row>
+    <row r="168" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN168" s="36"/>
+    </row>
+    <row r="169" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN169" s="36"/>
+    </row>
+    <row r="170" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN170" s="36"/>
+    </row>
+    <row r="171" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN171" s="36"/>
+    </row>
+    <row r="172" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN172" s="36"/>
+    </row>
+    <row r="173" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN173" s="36"/>
+    </row>
+    <row r="174" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN174" s="36"/>
+    </row>
+    <row r="175" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN175" s="36"/>
+    </row>
+    <row r="176" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN176" s="36"/>
+    </row>
+    <row r="177" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN177" s="36"/>
+    </row>
+    <row r="178" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN178" s="36"/>
+    </row>
+    <row r="179" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN179" s="36"/>
+    </row>
+    <row r="180" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN180" s="36"/>
+    </row>
+    <row r="181" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN181" s="36"/>
+    </row>
+    <row r="182" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN182" s="36"/>
+    </row>
+    <row r="183" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN183" s="36"/>
+    </row>
+    <row r="184" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN184" s="36"/>
+    </row>
+    <row r="185" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN185" s="36"/>
+    </row>
+    <row r="186" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN186" s="36"/>
+    </row>
+    <row r="187" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN187" s="36"/>
+    </row>
+    <row r="188" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN188" s="36"/>
+    </row>
+    <row r="189" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN189" s="36"/>
+    </row>
+    <row r="190" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN190" s="36"/>
+    </row>
+    <row r="191" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN191" s="36"/>
+    </row>
+    <row r="192" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN192" s="36"/>
+    </row>
+    <row r="193" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN193" s="36"/>
+    </row>
+    <row r="194" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN194" s="36"/>
+    </row>
+    <row r="195" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN195" s="36"/>
+    </row>
+    <row r="196" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN196" s="36"/>
+    </row>
+    <row r="197" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN197" s="36"/>
+    </row>
+    <row r="198" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN198" s="36"/>
+    </row>
+    <row r="199" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN199" s="36"/>
+    </row>
+    <row r="200" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN200" s="36"/>
+    </row>
+    <row r="201" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN201" s="36"/>
+    </row>
+    <row r="202" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN202" s="36"/>
+    </row>
+    <row r="203" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN203" s="36"/>
+    </row>
+    <row r="204" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN204" s="36"/>
+    </row>
+    <row r="205" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN205" s="36"/>
+    </row>
+    <row r="206" spans="40:40" x14ac:dyDescent="0.3">
+      <c r="AN206" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>